<commit_message>
(popis-dat) oprava excel šablony
</commit_message>
<xml_diff>
--- a/přílohy/popis-dat/šablony/Šablona-pro-popis-dat.xlsx
+++ b/přílohy/popis-dat/šablony/Šablona-pro-popis-dat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliceBinderová\data.gov.cz\přílohy\popis-dat\šablony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500DCFF-5BB7-49E3-A89E-20DE50797C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D577FEF-9DCD-46B2-ABB4-F6231986C12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slovník" sheetId="6" r:id="rId1"/>
@@ -739,15 +739,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC37FD07-DCA5-4F2E-BC5C-C20173B54937}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="59" customWidth="1"/>
-    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="2" max="2" width="75.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -755,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -789,22 +789,22 @@
       <selection pane="bottomRight" activeCell="F1" sqref="F1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1"/>
+    <col min="1" max="1" width="41.1796875" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" customWidth="1"/>
-    <col min="5" max="5" width="60.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="9" width="15.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" customWidth="1"/>
+    <col min="5" max="5" width="60.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="9" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
@@ -823,7 +823,7 @@
       </c>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -861,7 +861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -884,7 +884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -905,7 +905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -923,7 +923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -941,7 +941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -959,7 +959,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1016,32 +1016,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DDA33D-1F62-45BA-B8E5-510B45B31189}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" customWidth="1"/>
-    <col min="5" max="5" width="60.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
-    <col min="8" max="9" width="15.21875" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" customWidth="1"/>
+    <col min="5" max="5" width="60.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="9" width="15.1796875" customWidth="1"/>
+    <col min="11" max="11" width="16.453125" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="21.453125" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.6328125" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1163,31 +1163,31 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C14"/>
     </row>
   </sheetData>
@@ -1220,7 +1220,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Další, neoficiální název pojmu." sqref="H3:H1048576" xr:uid="{B93F9303-0069-48FD-B2F9-165E1F031165}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A2:XFD2" xr:uid="{B9B6ABAB-E396-4C2A-ACC5-4C9426BE2CE8}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1048576" xr:uid="{BD85CD45-49CC-44E4-A936-E7668DF670F4}">
-      <formula1>"Základních registrů,Jiných agend,Vlastní,Provozní"</formula1>
+      <formula1>"Nesdílené,Poskytované na žádost,Veřejně přístupné,Zpřístupňované pro výkon agendy"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Přiřazení do kategorie, která charakterizuje odpovídající údaj z hlediska způsobu jeho získání či vzniku v rámci dané věcné oblasti." sqref="O3:O1048576" xr:uid="{20C3A296-E413-4528-88FE-0B2E97CF88B5}">
       <formula1>"Základních registrů,Jiných agend,Vlastní,Provozní"</formula1>
@@ -1264,23 +1264,23 @@
       <selection pane="bottomRight" activeCell="O1" sqref="O1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" customWidth="1"/>
-    <col min="4" max="4" width="38.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5546875" customWidth="1"/>
-    <col min="6" max="6" width="60.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="10" width="15.21875" customWidth="1"/>
-    <col min="12" max="12" width="23.77734375" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="4" width="38.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" customWidth="1"/>
+    <col min="6" max="6" width="60.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="9" max="10" width="15.1796875" customWidth="1"/>
+    <col min="12" max="12" width="23.81640625" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1430,10 +1430,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D8"/>
     </row>
   </sheetData>
@@ -1488,6 +1488,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="295d819b-bf18-46bf-9ff7-08a644d34552">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003DFD27000E83C74CB14A0377F78F61D5" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="a9d78f77cf4282f25e3c937513c2cc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295d819b-bf18-46bf-9ff7-08a644d34552" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4670218af9848083cea27963b82eda20" ns2:_="">
     <xsd:import namespace="295d819b-bf18-46bf-9ff7-08a644d34552"/>
@@ -1665,26 +1684,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="295d819b-bf18-46bf-9ff7-08a644d34552">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61DD670D-BACE-46A4-9BA8-1B19F1BB41D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1700,28 +1724,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>